<commit_message>
visualization complete but wrong
</commit_message>
<xml_diff>
--- a/Vision Trajectory2.xlsx
+++ b/Vision Trajectory2.xlsx
@@ -42,7 +42,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +53,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -86,22 +92,22 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -413,30 +419,30 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -453,7 +459,7 @@
         <v>285.42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <f>A2+1/30</f>
       </c>
@@ -470,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <f>A3+1/30</f>
       </c>
@@ -487,7 +493,7 @@
         <v>382.324</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <f>A4+1/30</f>
       </c>
@@ -504,7 +510,7 @@
         <v>423.717</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <f>A5+1/30</f>
       </c>
@@ -521,7 +527,7 @@
         <v>461.97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <f>A6+1/30</f>
       </c>
@@ -538,7 +544,7 @@
         <v>494.068</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <f>A7+1/30</f>
       </c>
@@ -555,7 +561,7 @@
         <v>518.07</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <f>A8+1/30</f>
       </c>
@@ -572,7 +578,7 @@
         <v>539.766</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <f>A9+1/30</f>
       </c>
@@ -589,7 +595,7 @@
         <v>560.658</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <f>A10+1/30</f>
       </c>
@@ -606,7 +612,7 @@
         <v>578.837</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <f>A11+1/30</f>
       </c>
@@ -623,7 +629,7 @@
         <v>593.609</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <f>A12+1/30</f>
       </c>
@@ -640,7 +646,7 @@
         <v>605.716</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <f>A13+1/30</f>
       </c>
@@ -657,7 +663,7 @@
         <v>616.974</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <f>A14+1/30</f>
       </c>
@@ -674,7 +680,7 @@
         <v>627.425</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <f>A15+1/30</f>
       </c>
@@ -691,7 +697,7 @@
         <v>638.688</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <f>A16+1/30</f>
       </c>
@@ -1422,26 +1428,26 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2499,26 +2505,26 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3542,26 +3548,26 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>